<commit_message>
amélioration rep eta, N, config
</commit_message>
<xml_diff>
--- a/Analyse_de_lalgo.xlsx
+++ b/Analyse_de_lalgo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\kohonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EFDB9E-6153-4FB9-B644-C2FDBABBAF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F49786-154E-49FD-92B7-A7CB09EF0D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{0A90DB37-95E1-41D2-AF98-710D4518E643}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{0A90DB37-95E1-41D2-AF98-710D4518E643}"/>
   </bookViews>
   <sheets>
     <sheet name="Variation eta" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>sigma</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>erreur de quantification</t>
+  </si>
+  <si>
+    <t>coef de resserement</t>
+  </si>
+  <si>
+    <t>Distribution d’entrée</t>
   </si>
 </sst>
 </file>
@@ -137,7 +143,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1382,26 +1388,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1410,8 +1396,1140 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="8"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>erreur de quantification vectorielle moyenne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>erreur de quantification vectorielle moyenne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000014-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>erreur de quantification vectorielle moyenne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000015-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000016-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>erreur de quantification vectorielle moyenne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000017-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>erreur de quantification vectorielle moyenne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>erreur de quantification vectorielle moyenne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>erreur de quantification vectorielle moyenne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.34530902747472197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30508922396736698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.113894495582435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4733723450160701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3280553881144699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.28478016454498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-E929-41E1-AC46-EB9B7321E921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="14"/>
           <c:tx>
             <c:strRef>
               <c:f>'Evolution N'!$A$1</c:f>
@@ -1481,22 +2599,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.367120145568056</c:v>
+                  <c:v>0.34530902747472197</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32234571435660703</c:v>
+                  <c:v>0.30508922396736698</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15405690041176401</c:v>
+                  <c:v>0.113894495582435</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3080105189364502E-2</c:v>
+                  <c:v>3.4733723450160701E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9243282630186501E-2</c:v>
+                  <c:v>1.3280553881144699E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.26151775102828E-2</c:v>
+                  <c:v>1.28478016454498E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1504,13 +2622,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9179-4AC8-9A1F-35E48F758F7B}"/>
+              <c16:uniqueId val="{0000000D-E929-41E1-AC46-EB9B7321E921}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="15"/>
           <c:tx>
             <c:strRef>
               <c:f>'Evolution N'!$B$1</c:f>
@@ -1580,22 +2698,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.367120145568056</c:v>
+                  <c:v>0.34530902747472197</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32234571435660703</c:v>
+                  <c:v>0.30508922396736698</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15405690041176401</c:v>
+                  <c:v>0.113894495582435</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3080105189364502E-2</c:v>
+                  <c:v>3.4733723450160701E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9243282630186501E-2</c:v>
+                  <c:v>1.3280553881144699E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.26151775102828E-2</c:v>
+                  <c:v>1.28478016454498E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1603,7 +2721,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9179-4AC8-9A1F-35E48F758F7B}"/>
+              <c16:uniqueId val="{0000000F-E929-41E1-AC46-EB9B7321E921}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1724,6 +2842,423 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="202388479"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>coef de resserement</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>coef de resserement</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.139801809174799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.631211059919494</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.951245303789001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.664847603013699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.16207598200572</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7258438011565902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F89C-41FB-B1D2-9E80A0284646}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Evolution N'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>coef de resserement</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Evolution N'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Evolution N'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.139801809174799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.631211059919494</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.951245303789001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.664847603013699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.16207598200572</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7258438011565902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F89C-41FB-B1D2-9E80A0284646}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="379950367"/>
+        <c:axId val="379957087"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="379950367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379957087"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="379957087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379950367"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4117,16 +5652,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4146,6 +5681,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DFCB989-609C-A7DB-AEF1-F316782DE2F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4453,8 +6024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2907D987-5374-4FE4-AD7C-107A7DCEA878}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4538,7 +6109,7 @@
   <dimension ref="E6:F13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5020,77 +6591,101 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB0FD98-DFC0-4B6B-BDFE-FFBA405C649E}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="22" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>0.367120145568056</v>
+        <v>0.34530902747472197</v>
+      </c>
+      <c r="C2" s="2">
+        <v>53.139801809174799</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>0.32234571435660703</v>
+        <v>0.30508922396736698</v>
+      </c>
+      <c r="C3" s="2">
+        <v>67.631211059919494</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>100</v>
       </c>
       <c r="B4" s="2">
-        <v>0.15405690041176401</v>
+        <v>0.113894495582435</v>
+      </c>
+      <c r="C4" s="2">
+        <v>41.951245303789001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1000</v>
       </c>
       <c r="B5" s="2">
-        <v>3.3080105189364502E-2</v>
+        <v>3.4733723450160701E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>14.664847603013699</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>10000</v>
       </c>
       <c r="B6" s="2">
-        <v>1.9243282630186501E-2</v>
+        <v>1.3280553881144699E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6.16207598200572</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>100000</v>
       </c>
       <c r="B7" s="2">
-        <v>1.26151775102828E-2</v>
+        <v>1.28478016454498E-2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5.7258438011565902</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5098,8 +6693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966E2810-1735-418A-B4BB-D220D0DF4604}">
   <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5110,18 +6705,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>1.34736930625141E-2</v>
       </c>
       <c r="D3" s="6">
@@ -5129,24 +6727,24 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1.15286452796692E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>5.7632439675614702</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>9.4505826206386003E-3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>6.9817690370148204</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mise en page partie 1 et 2
</commit_message>
<xml_diff>
--- a/Analyse_de_lalgo.xlsx
+++ b/Analyse_de_lalgo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\kohonen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C72682\Documents\GitHub\kohonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F49786-154E-49FD-92B7-A7CB09EF0D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C15A17-2586-4E5C-9EB2-D3A12C32514F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{0A90DB37-95E1-41D2-AF98-710D4518E643}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{0A90DB37-95E1-41D2-AF98-710D4518E643}"/>
   </bookViews>
   <sheets>
     <sheet name="Variation eta" sheetId="3" r:id="rId1"/>
@@ -24,12 +24,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>sigma</t>
   </si>
@@ -80,6 +91,15 @@
   </si>
   <si>
     <t>Distribution d’entrée</t>
+  </si>
+  <si>
+    <t>[−1, 1] × [−1, 1] et 3* [0, 1] x [0, 1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[−1, 0] × [-1, 1] et 3*[0, 1] × [-1, 1] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[−1, 0] × [-1, 1] et 7*[0, 1] × [-1, 1] </t>
   </si>
 </sst>
 </file>
@@ -6024,7 +6044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2907D987-5374-4FE4-AD7C-107A7DCEA878}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -6100,7 +6120,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6174,7 +6195,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6585,7 +6607,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6691,17 +6714,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966E2810-1735-418A-B4BB-D220D0DF4604}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="41.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -6746,6 +6771,39 @@
       </c>
       <c r="D5" s="2">
         <v>6.9817690370148204</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.3693043211208801E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5.5910500134726098</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.6174594770509799E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5.1341867715500697</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.5226258240725101E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.6756390201862503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
suite de la réponse partie 3
</commit_message>
<xml_diff>
--- a/Analyse_de_lalgo.xlsx
+++ b/Analyse_de_lalgo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C72682\Documents\GitHub\kohonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C15A17-2586-4E5C-9EB2-D3A12C32514F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4618C87C-0619-4D0F-9022-ED83F3F61C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{0A90DB37-95E1-41D2-AF98-710D4518E643}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{0A90DB37-95E1-41D2-AF98-710D4518E643}"/>
   </bookViews>
   <sheets>
     <sheet name="Variation eta" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Evolution exponentielle" sheetId="2" r:id="rId3"/>
     <sheet name="Evolution N" sheetId="4" r:id="rId4"/>
     <sheet name="Evolution distribution" sheetId="5" r:id="rId5"/>
+    <sheet name="calcul main (2,2)" sheetId="6" r:id="rId6"/>
+    <sheet name="calcul main (rand,rand)" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>sigma</t>
   </si>
@@ -101,12 +103,66 @@
   <si>
     <t xml:space="preserve">[−1, 0] × [-1, 1] et 7*[0, 1] × [-1, 1] </t>
   </si>
+  <si>
+    <t>algo</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>v2 moyenne de 5 valeurs</t>
+  </si>
+  <si>
+    <t>v2 moyenne de 3 valeurs</t>
+  </si>
+  <si>
+    <t>v3 moyenne de 5 valeurs</t>
+  </si>
+  <si>
+    <t>v3 moyenne de 3 valeurs</t>
+  </si>
+  <si>
+    <t>Ecart test 1</t>
+  </si>
+  <si>
+    <t>Ecart test 2</t>
+  </si>
+  <si>
+    <t>Ecart test 3</t>
+  </si>
+  <si>
+    <t>Ecart test 4</t>
+  </si>
+  <si>
+    <t>Ecart test 5</t>
+  </si>
+  <si>
+    <t>Ecart test 6</t>
+  </si>
+  <si>
+    <t>Ecart test 7</t>
+  </si>
+  <si>
+    <t>Ecart test 8</t>
+  </si>
+  <si>
+    <t>Ecart test 9</t>
+  </si>
+  <si>
+    <t>Ecart test 10</t>
+  </si>
+  <si>
+    <t>Avec la co fixe (2,2)</t>
+  </si>
+  <si>
+    <t>Avec la co random</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +178,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3334,6 +3396,1732 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (2,2)'!$C$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.7145100000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0490159999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1717400000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6687650000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5090399999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0742150000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.277901E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11369303</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2943959999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4506480000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F1EB-456D-BB51-981E2CFBA58D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v2 moyenne de 5 valeurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (2,2)'!$C$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.865031E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.776848E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9098170000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5142329999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7717010000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7956769999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7539530000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.9342929999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6998739999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7552749999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F1EB-456D-BB51-981E2CFBA58D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v2 moyenne de 3 valeurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (2,2)'!$C$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.1147689999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.952948E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.163965E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5558640000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2483999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.499002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3884800000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.484268E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0785709999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.519573E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F1EB-456D-BB51-981E2CFBA58D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v3 moyenne de 5 valeurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (2,2)'!$C$6:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.769772E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.806205E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7596870000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4781909999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.296425E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.625299E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5818490000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0322400000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.517755E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.764392E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F1EB-456D-BB51-981E2CFBA58D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v3 moyenne de 3 valeurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (2,2)'!$C$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.2859000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8684950000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2576899999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3999969999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7768799999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.526886E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8610580000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.6612640000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2846929999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4748220000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F1EB-456D-BB51-981E2CFBA58D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1044150696"/>
+        <c:axId val="1044146376"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1044150696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1044146376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1044146376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1044150696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (rand,rand)'!$C$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.5487530000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0782419999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7741810000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5243740000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.214356E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.61835E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4967679999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5722399999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7782439999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2106160000000002E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1C65-4D02-8E18-B5F17614B751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v2 moyenne de 5 valeurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (rand,rand)'!$C$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.2124E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.311724E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8422200000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1869400000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.132172E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9758719999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3348700000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2930559999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9815100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2696709999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1C65-4D02-8E18-B5F17614B751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v2 moyenne de 3 valeurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (rand,rand)'!$C$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.9841100000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.124058E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5032199999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4956679999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.37793E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0713620000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8900599999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.6184500000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.6029499999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8924209999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1C65-4D02-8E18-B5F17614B751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v3 moyenne de 5 valeurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (rand,rand)'!$C$6:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.7663190000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.271104E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0201500000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.183068E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.117741E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5105309999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6408999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8532709999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3317300000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1388919999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1C65-4D02-8E18-B5F17614B751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v3 moyenne de 3 valeurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'calcul main (rand,rand)'!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Ecart test 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ecart test 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ecart test 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ecart test 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ecart test 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ecart test 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ecart test 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ecart test 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ecart test 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ecart test 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'calcul main (rand,rand)'!$C$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.4936100000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0424360000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3862399999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.566972E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.70785E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6311640000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.78335E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3998500000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1718399999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5799539999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1C65-4D02-8E18-B5F17614B751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="315864768"/>
+        <c:axId val="315873408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="315864768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="315873408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="315873408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="315864768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3494,6 +5282,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5043,6 +6911,1012 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5745,6 +8619,88 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>827325</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>138525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{474AD4B8-9DE0-74ED-98B5-ABDFD2CDD353}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47623</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>865423</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>157576</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5C31EFC-E680-0C00-09FF-3009E5A21D50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -6716,7 +9672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966E2810-1735-418A-B4BB-D220D0DF4604}">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -6810,4 +9766,479 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBD9C8D-75E4-4F08-BC46-E454B50455B6}">
+  <dimension ref="B2:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="12" width="18.7109375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2">
+        <v>9.7145100000000009E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.0490159999999999E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.1717400000000002E-3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3.6687650000000002E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>9.5090399999999999E-3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2.0742150000000001E-2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.277901E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.11369303</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.2943959999999999E-2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>5.4506480000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.865031E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.776848E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.9098170000000001E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.5142329999999999E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3.7717010000000002E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2.7956769999999999E-2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.7539530000000001E-2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3.9342929999999998E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1.6998739999999998E-2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.7552749999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.1147689999999999E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.952948E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.163965E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.5558640000000002E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3.2483999999999998E-3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.499002E-2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2.3884800000000001E-2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>6.484268E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.0785709999999999E-2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2.519573E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.769772E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.806205E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.7596870000000001E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3.4781909999999999E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3.296425E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2.625299E-2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1.5818490000000001E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4.0322400000000001E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1.517755E-2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1.764392E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.2859000000000001E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.8684950000000001E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8.2576899999999998E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3.3999969999999997E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2.7768799999999998E-3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.526886E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.8610580000000002E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>6.6612640000000001E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1.2846929999999999E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2.4748220000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6903C6-35CA-4E7A-B917-D32060D0F9C9}">
+  <dimension ref="B2:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="12" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.5487530000000001E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>8.0782419999999994E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.7741810000000001E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.5243740000000001E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.214356E-2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.61835E-2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2.4967679999999999E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2.5722399999999999E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2.7782439999999999E-2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>3.2106160000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.2124E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.311724E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7.8422200000000004E-3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>8.1869400000000002E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.132172E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2.9758719999999999E-2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>6.3348700000000003E-3</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3.2930559999999998E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1.9815100000000001E-3</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2.2696709999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7.9841100000000009E-3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.124058E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.5032199999999996E-3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.4956679999999998E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.37793E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3.0713620000000001E-2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6.8900599999999999E-3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>9.6184500000000006E-3</v>
+      </c>
+      <c r="K5" s="2">
+        <v>7.6029499999999998E-3</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2.8924209999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.7663190000000001E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.271104E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7.0201500000000002E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.183068E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.117741E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2.5105309999999999E-2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>6.6408999999999999E-3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2.8532709999999999E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2.3317300000000002E-3</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2.1388919999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7.4936100000000004E-3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.0424360000000001E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5.3862399999999996E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.566972E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.70785E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2.6311640000000001E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2.78335E-3</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5.3998500000000003E-3</v>
+      </c>
+      <c r="K7" s="2">
+        <v>8.1718399999999997E-3</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2.5799539999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fin question sur le bras
</commit_message>
<xml_diff>
--- a/Analyse_de_lalgo.xlsx
+++ b/Analyse_de_lalgo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C72682\Documents\GitHub\kohonen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\code\kohonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4618C87C-0619-4D0F-9022-ED83F3F61C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5DBA20-70C3-42C2-8C44-0A69E1A42D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{0A90DB37-95E1-41D2-AF98-710D4518E643}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="5" xr2:uid="{0A90DB37-95E1-41D2-AF98-710D4518E643}"/>
   </bookViews>
   <sheets>
     <sheet name="Variation eta" sheetId="3" r:id="rId1"/>
@@ -18,8 +18,7 @@
     <sheet name="Evolution exponentielle" sheetId="2" r:id="rId3"/>
     <sheet name="Evolution N" sheetId="4" r:id="rId4"/>
     <sheet name="Evolution distribution" sheetId="5" r:id="rId5"/>
-    <sheet name="calcul main (2,2)" sheetId="6" r:id="rId6"/>
-    <sheet name="calcul main (rand,rand)" sheetId="7" r:id="rId7"/>
+    <sheet name="calcul main (rand,rand)" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>sigma</t>
   </si>
@@ -104,22 +103,7 @@
     <t xml:space="preserve">[−1, 0] × [-1, 1] et 7*[0, 1] × [-1, 1] </t>
   </si>
   <si>
-    <t>algo</t>
-  </si>
-  <si>
     <t>v1</t>
-  </si>
-  <si>
-    <t>v2 moyenne de 5 valeurs</t>
-  </si>
-  <si>
-    <t>v2 moyenne de 3 valeurs</t>
-  </si>
-  <si>
-    <t>v3 moyenne de 5 valeurs</t>
-  </si>
-  <si>
-    <t>v3 moyenne de 3 valeurs</t>
   </si>
   <si>
     <t>Ecart test 1</t>
@@ -152,10 +136,10 @@
     <t>Ecart test 10</t>
   </si>
   <si>
-    <t>Avec la co fixe (2,2)</t>
+    <t>v2 moyenne de 4 neuronnes</t>
   </si>
   <si>
-    <t>Avec la co random</t>
+    <t xml:space="preserve">v3 moyenne de 4 neuronnes </t>
   </si>
 </sst>
 </file>
@@ -183,10 +167,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -226,6 +209,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3411,694 +3397,13 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Ecart test 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ecart test 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ecart test 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ecart test 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Ecart test 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Ecart test 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Ecart test 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ecart test 8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Ecart test 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ecart test 10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'calcul main (2,2)'!$C$3:$L$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>9.7145100000000009E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.0490159999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.1717400000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.6687650000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.5090399999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.0742150000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.277901E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.11369303</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.2943959999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.4506480000000003E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F1EB-456D-BB51-981E2CFBA58D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v2 moyenne de 5 valeurs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Ecart test 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ecart test 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ecart test 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ecart test 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Ecart test 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Ecart test 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Ecart test 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ecart test 8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Ecart test 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ecart test 10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'calcul main (2,2)'!$C$4:$L$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1.865031E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.776848E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9098170000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.5142329999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.7717010000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.7956769999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7539530000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.9342929999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.6998739999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7552749999999999E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F1EB-456D-BB51-981E2CFBA58D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v2 moyenne de 3 valeurs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Ecart test 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ecart test 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ecart test 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ecart test 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Ecart test 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Ecart test 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Ecart test 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ecart test 8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Ecart test 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ecart test 10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'calcul main (2,2)'!$C$5:$L$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>3.1147689999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.952948E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.163965E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.5558640000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2483999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.499002E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.3884800000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.484268E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.0785709999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.519573E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F1EB-456D-BB51-981E2CFBA58D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v3 moyenne de 5 valeurs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Ecart test 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ecart test 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ecart test 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ecart test 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Ecart test 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Ecart test 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Ecart test 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ecart test 8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Ecart test 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ecart test 10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'calcul main (2,2)'!$C$6:$L$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1.769772E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.806205E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7596870000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.4781909999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.296425E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.625299E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5818490000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.0322400000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.517755E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.764392E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F1EB-456D-BB51-981E2CFBA58D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v3 moyenne de 3 valeurs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'calcul main (2,2)'!$C$2:$L$2</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Ecart test 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ecart test 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ecart test 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ecart test 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Ecart test 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Ecart test 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Ecart test 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ecart test 8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Ecart test 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ecart test 10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'calcul main (2,2)'!$C$7:$L$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2.2859000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.8684950000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.2576899999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.3999969999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.7768799999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.526886E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.8610580000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.6612640000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.2846929999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.4748220000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-F1EB-456D-BB51-981E2CFBA58D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1044150696"/>
-        <c:axId val="1044146376"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1044150696"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4110,170 +3415,18 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Comparaison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> des distance par rapport à l'ideal des solutions V1, V2 et V3</a:t>
+            </a:r>
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
-        </c:txPr>
-        <c:crossAx val="1044146376"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1044146376"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1044150696"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4392,34 +3545,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.5487530000000001E-2</c:v>
+                  <c:v>0.14314023916904001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0782419999999994E-2</c:v>
+                  <c:v>7.24718772295493E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7741810000000001E-2</c:v>
+                  <c:v>0.110684845351599</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5243740000000001E-2</c:v>
+                  <c:v>0.102162280418993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.214356E-2</c:v>
+                  <c:v>7.2316192708528598E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.61835E-2</c:v>
+                  <c:v>0.108170665814785</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4967679999999999E-2</c:v>
+                  <c:v>1.4783490908512E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5722399999999999E-2</c:v>
+                  <c:v>9.4939985949541797E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7782439999999999E-2</c:v>
+                  <c:v>3.48223675952785E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2106160000000002E-2</c:v>
+                  <c:v>3.09629632413887E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4440,7 +3593,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v2 moyenne de 5 valeurs</c:v>
+                  <c:v>v2 moyenne de 4 neuronnes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4514,34 +3667,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.2124E-2</c:v>
+                  <c:v>8.5742064294131504E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.311724E-2</c:v>
+                  <c:v>2.38195413118268E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8422200000000004E-3</c:v>
+                  <c:v>6.51429457985154E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1869400000000002E-3</c:v>
+                  <c:v>0.13975161815516099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.132172E-2</c:v>
+                  <c:v>9.9254452120439096E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9758719999999999E-2</c:v>
+                  <c:v>4.0782534561016798E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3348700000000003E-3</c:v>
+                  <c:v>2.50062060391661E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.2930559999999998E-2</c:v>
+                  <c:v>5.65665722067102E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9815100000000001E-3</c:v>
+                  <c:v>3.6307011443075E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.2696709999999998E-2</c:v>
+                  <c:v>4.9778992920341499E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4554,7 +3707,7 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="4"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
@@ -4562,251 +3715,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v2 moyenne de 3 valeurs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'calcul main (rand,rand)'!$C$2:$L$2</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Ecart test 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ecart test 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ecart test 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ecart test 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Ecart test 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Ecart test 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Ecart test 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ecart test 8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Ecart test 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ecart test 10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'calcul main (rand,rand)'!$C$5:$L$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>7.9841100000000009E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.124058E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.5032199999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.4956679999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.37793E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.0713620000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.8900599999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.6184500000000006E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.6029499999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.8924209999999999E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1C65-4D02-8E18-B5F17614B751}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'calcul main (rand,rand)'!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v3 moyenne de 5 valeurs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'calcul main (rand,rand)'!$C$2:$L$2</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Ecart test 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ecart test 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ecart test 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ecart test 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Ecart test 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Ecart test 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Ecart test 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ecart test 8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Ecart test 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ecart test 10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'calcul main (rand,rand)'!$C$6:$L$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2.7663190000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.271104E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.0201500000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.183068E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.117741E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5105309999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.6408999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.8532709999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.3317300000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.1388919999999999E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-1C65-4D02-8E18-B5F17614B751}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'calcul main (rand,rand)'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v3 moyenne de 3 valeurs</c:v>
+                  <c:v>v3 moyenne de 4 neuronnes </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4875,39 +3784,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'calcul main (rand,rand)'!$C$7:$L$7</c:f>
+              <c:f>'calcul main (rand,rand)'!$C$5:$L$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7.4936100000000004E-3</c:v>
+                  <c:v>8.28044700853688E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0424360000000001E-2</c:v>
+                  <c:v>2.35894172826146E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3862399999999996E-3</c:v>
+                  <c:v>6.4601930282148404E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.566972E-2</c:v>
+                  <c:v>0.13190799017809901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.70785E-2</c:v>
+                  <c:v>9.4839073164124599E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6311640000000001E-2</c:v>
+                  <c:v>3.9636654316615998E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.78335E-3</c:v>
+                  <c:v>2.4385823199888901E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3998500000000003E-3</c:v>
+                  <c:v>4.5974071534220402E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.1718399999999997E-3</c:v>
+                  <c:v>3.54266520132306E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5799539999999999E-2</c:v>
+                  <c:v>4.5673552887832897E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5322,46 +4231,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7414,509 +6283,6 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8624,55 +6990,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>827325</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>138525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Graphique 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{474AD4B8-9DE0-74ED-98B5-ABDFD2CDD353}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>47623</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>865423</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>157576</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8702,9 +7027,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8742,7 +7067,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8848,7 +7173,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8990,7 +7315,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9769,250 +8094,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBD9C8D-75E4-4F08-BC46-E454B50455B6}">
-  <dimension ref="B2:L10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="12" width="18.7109375" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9.7145100000000009E-3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3.0490159999999999E-2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>7.1717400000000002E-3</v>
-      </c>
-      <c r="F3" s="2">
-        <v>3.6687650000000002E-2</v>
-      </c>
-      <c r="G3" s="2">
-        <v>9.5090399999999999E-3</v>
-      </c>
-      <c r="H3" s="2">
-        <v>2.0742150000000001E-2</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1.277901E-2</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.11369303</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1.2943959999999999E-2</v>
-      </c>
-      <c r="L3" s="2">
-        <v>5.4506480000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.865031E-2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.776848E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.9098170000000001E-2</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3.5142329999999999E-2</v>
-      </c>
-      <c r="G4" s="2">
-        <v>3.7717010000000002E-2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2.7956769999999999E-2</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1.7539530000000001E-2</v>
-      </c>
-      <c r="J4" s="2">
-        <v>3.9342929999999998E-2</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1.6998739999999998E-2</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1.7552749999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3.1147689999999999E-2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2.952948E-2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.163965E-2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>3.5558640000000002E-2</v>
-      </c>
-      <c r="G5" s="2">
-        <v>3.2483999999999998E-3</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1.499002E-2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>2.3884800000000001E-2</v>
-      </c>
-      <c r="J5" s="2">
-        <v>6.484268E-2</v>
-      </c>
-      <c r="K5" s="2">
-        <v>2.0785709999999999E-2</v>
-      </c>
-      <c r="L5" s="2">
-        <v>2.519573E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.769772E-2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.806205E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.7596870000000001E-2</v>
-      </c>
-      <c r="F6" s="2">
-        <v>3.4781909999999999E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <v>3.296425E-2</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2.625299E-2</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1.5818490000000001E-2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>4.0322400000000001E-2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1.517755E-2</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1.764392E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2.2859000000000001E-2</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2.8684950000000001E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>8.2576899999999998E-3</v>
-      </c>
-      <c r="F7" s="2">
-        <v>3.3999969999999997E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2.7768799999999998E-3</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1.526886E-2</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1.8610580000000002E-2</v>
-      </c>
-      <c r="J7" s="2">
-        <v>6.6612640000000001E-2</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1.2846929999999999E-2</v>
-      </c>
-      <c r="L7" s="2">
-        <v>2.4748220000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6903C6-35CA-4E7A-B917-D32060D0F9C9}">
-  <dimension ref="B2:L9"/>
+  <dimension ref="B2:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10022,219 +8108,145 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="J2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="K2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="L2" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2.5487530000000001E-2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>8.0782419999999994E-2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3.7741810000000001E-2</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2.5243740000000001E-2</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2.214356E-2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1.61835E-2</v>
-      </c>
-      <c r="I3" s="2">
-        <v>2.4967679999999999E-2</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2.5722399999999999E-2</v>
-      </c>
-      <c r="K3" s="2">
-        <v>2.7782439999999999E-2</v>
-      </c>
-      <c r="L3" s="2">
-        <v>3.2106160000000002E-2</v>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.14314023916904001</v>
+      </c>
+      <c r="D3" s="7">
+        <v>7.24718772295493E-2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.110684845351599</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.102162280418993</v>
+      </c>
+      <c r="G3" s="7">
+        <v>7.2316192708528598E-2</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.108170665814785</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1.4783490908512E-2</v>
+      </c>
+      <c r="J3" s="7">
+        <v>9.4939985949541797E-2</v>
+      </c>
+      <c r="K3" s="7">
+        <v>3.48223675952785E-2</v>
+      </c>
+      <c r="L3" s="7">
+        <v>3.09629632413887E-2</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3.2124E-2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.311724E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>7.8422200000000004E-3</v>
-      </c>
-      <c r="F4" s="2">
-        <v>8.1869400000000002E-3</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1.132172E-2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2.9758719999999999E-2</v>
-      </c>
-      <c r="I4" s="2">
-        <v>6.3348700000000003E-3</v>
-      </c>
-      <c r="J4" s="2">
-        <v>3.2930559999999998E-2</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1.9815100000000001E-3</v>
-      </c>
-      <c r="L4" s="2">
-        <v>2.2696709999999998E-2</v>
+      <c r="B4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="7">
+        <v>8.5742064294131504E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2.38195413118268E-2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>6.51429457985154E-2</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.13975161815516099</v>
+      </c>
+      <c r="G4" s="7">
+        <v>9.9254452120439096E-2</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4.0782534561016798E-2</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2.50062060391661E-2</v>
+      </c>
+      <c r="J4" s="7">
+        <v>5.65665722067102E-2</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3.6307011443075E-2</v>
+      </c>
+      <c r="L4" s="7">
+        <v>4.9778992920341499E-2</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2">
-        <v>7.9841100000000009E-3</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.124058E-2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5.5032199999999996E-3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2.4956679999999998E-2</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1.37793E-2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>3.0713620000000001E-2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>6.8900599999999999E-3</v>
-      </c>
-      <c r="J5" s="2">
-        <v>9.6184500000000006E-3</v>
-      </c>
-      <c r="K5" s="2">
-        <v>7.6029499999999998E-3</v>
-      </c>
-      <c r="L5" s="2">
-        <v>2.8924209999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2.7663190000000001E-2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.271104E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>7.0201500000000002E-3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.183068E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1.117741E-2</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2.5105309999999999E-2</v>
-      </c>
-      <c r="I6" s="2">
-        <v>6.6408999999999999E-3</v>
-      </c>
-      <c r="J6" s="2">
-        <v>2.8532709999999999E-2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2.3317300000000002E-3</v>
-      </c>
-      <c r="L6" s="2">
-        <v>2.1388919999999999E-2</v>
+      <c r="B5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="7">
+        <v>8.28044700853688E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2.35894172826146E-2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>6.4601930282148404E-2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.13190799017809901</v>
+      </c>
+      <c r="G5" s="7">
+        <v>9.4839073164124599E-2</v>
+      </c>
+      <c r="H5" s="7">
+        <v>3.9636654316615998E-2</v>
+      </c>
+      <c r="I5" s="7">
+        <v>2.4385823199888901E-2</v>
+      </c>
+      <c r="J5" s="7">
+        <v>4.5974071534220402E-2</v>
+      </c>
+      <c r="K5" s="7">
+        <v>3.54266520132306E-2</v>
+      </c>
+      <c r="L5" s="7">
+        <v>4.5673552887832897E-2</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2">
-        <v>7.4936100000000004E-3</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0424360000000001E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5.3862399999999996E-3</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2.566972E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1.70785E-2</v>
-      </c>
-      <c r="H7" s="2">
-        <v>2.6311640000000001E-2</v>
-      </c>
-      <c r="I7" s="2">
-        <v>2.78335E-3</v>
-      </c>
-      <c r="J7" s="2">
-        <v>5.3998500000000003E-3</v>
-      </c>
-      <c r="K7" s="2">
-        <v>8.1718399999999997E-3</v>
-      </c>
-      <c r="L7" s="2">
-        <v>2.5799539999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>